<commit_message>
evaluate rosindex and google
</commit_message>
<xml_diff>
--- a/pkg_recommendation/evaluation-task.xlsx
+++ b/pkg_recommendation/evaluation-task.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27100" windowHeight="13220" tabRatio="995" activeTab="1"/>
+    <workbookView windowWidth="23400" windowHeight="17040" tabRatio="995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="22">
   <si>
     <t>task number</t>
   </si>
@@ -66,16 +66,22 @@
     <t>top1</t>
   </si>
   <si>
-    <t>top3</t>
-  </si>
-  <si>
     <t>top5</t>
   </si>
   <si>
     <t>top10</t>
   </si>
   <si>
+    <t>top15</t>
+  </si>
+  <si>
+    <t>top20</t>
+  </si>
+  <si>
     <t>query-id</t>
+  </si>
+  <si>
+    <t>rosindex check</t>
   </si>
 </sst>
 </file>
@@ -83,10 +89,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -96,30 +102,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,45 +117,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,15 +177,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,23 +194,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,6 +210,43 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,25 +261,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,31 +291,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,43 +315,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,13 +327,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,31 +363,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,6 +403,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -446,30 +452,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -497,11 +479,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,6 +511,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -533,154 +530,163 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1007,8 +1013,8 @@
   <sheetPr/>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.2" outlineLevelCol="7"/>
@@ -1166,7 +1172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1182,15 +1188,39 @@
       <c r="E24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>0.33</v>
+      </c>
+      <c r="C25">
+        <v>0.45</v>
+      </c>
+      <c r="D25">
+        <v>0.49</v>
+      </c>
+      <c r="E25">
+        <v>0.51</v>
+      </c>
+      <c r="F25">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>4</v>
+      </c>
+      <c r="B26">
+        <v>0.07</v>
+      </c>
+      <c r="C26">
+        <v>0.14</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -1221,17 +1251,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="138" zoomScaleNormal="138" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1248,1105 +1278,2731 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2">
+        <v>194</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(H2&gt;19,"NA",H2+1)</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
       <c r="F3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <v>199</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I34" si="0">IF(H3&gt;19,"NA",H3+1)</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4">
+        <v>319</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7">
+        <v>64</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8">
+        <v>51</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
       <c r="F9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9">
+        <v>179</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="F10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10">
+        <v>132</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11">
+        <v>96</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12">
+        <v>201</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13">
+        <v>66</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>11</v>
       </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15">
+        <v>493</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16">
+        <v>123</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
       <c r="F17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17">
+        <v>25</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
       <c r="F18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18">
+        <v>62</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
       <c r="F19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
       <c r="F20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23">
+        <v>24</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="H25">
+        <v>175</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
       <c r="F26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="H26">
+        <v>69</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
       <c r="F27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="H27">
+        <v>107</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="H28">
+        <v>25</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="H29">
+        <v>116</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
       <c r="F30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="H30">
+        <v>134</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
       <c r="F31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="H31">
+        <v>77</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
       <c r="F32">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="H32">
+        <v>141</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
       <c r="F33">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="H33">
+        <v>207</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
       <c r="F34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="H34">
+        <v>12</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>11</v>
+      </c>
       <c r="F35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:I66" si="1">IF(H35&gt;19,"NA",H35+1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
       <c r="F37">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="H37">
+        <v>7</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
       </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
       <c r="F38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="H38">
+        <v>46</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
       <c r="F39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="H39">
+        <v>68</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
       <c r="F41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="H41">
+        <v>41</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
       <c r="F42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="H42">
+        <v>12</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
       <c r="F43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
       <c r="F44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
       <c r="F45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
       <c r="F46">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
       <c r="F47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="H47" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
       <c r="F48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="H48">
+        <v>3</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>6</v>
+      </c>
       <c r="F49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
       <c r="F50">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="H50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <v>11</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="H51">
+        <v>10</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
       <c r="F52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
       <c r="F53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
       <c r="F54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="H54" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
       <c r="F55">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
       <c r="F56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="H56">
+        <v>157</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
       <c r="F57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="H57">
+        <v>24</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
       <c r="F58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
       <c r="F59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="H59">
+        <v>37</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
       <c r="F60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="H60">
+        <v>331</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
       <c r="F61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="H61">
+        <v>211</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
       <c r="F62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="H62">
+        <v>29</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
       <c r="F63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64">
+        <v>13</v>
+      </c>
       <c r="F64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="H64" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
         <v>4</v>
       </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
       <c r="F65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="H65" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
       <c r="F66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="H66" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
       <c r="F67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="H67">
+        <v>51</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I98" si="2">IF(H67&gt;19,"NA",H67+1)</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
       <c r="F68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="H68" t="s">
+        <v>9</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69">
+        <v>7</v>
+      </c>
       <c r="F69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="H69">
+        <v>215</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
         <v>6</v>
       </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
       <c r="F70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="H70">
+        <v>50</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
       </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
       <c r="F71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="H71" t="s">
+        <v>9</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
       <c r="F72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="H72">
+        <v>57</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
         <v>13</v>
       </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73">
+        <v>11</v>
+      </c>
+      <c r="E73">
+        <v>4</v>
+      </c>
       <c r="F73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="H73">
+        <v>10</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
       </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
       <c r="F74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="H74">
+        <v>191</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
       <c r="F75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="H75" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
       <c r="F76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="H76" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
         <v>4</v>
       </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
       <c r="F77" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="H77">
+        <v>25</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
       </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78">
+        <v>16</v>
+      </c>
       <c r="F78" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="H78">
+        <v>22</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79">
+        <v>8</v>
+      </c>
       <c r="F79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="H79" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
       </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
       <c r="F80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="H80">
+        <v>21</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
       <c r="F81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="H81" t="s">
+        <v>9</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
       <c r="F82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="H82">
+        <v>178</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
       <c r="F83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="H83">
+        <v>51</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
       </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
       <c r="F84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="H84" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
       <c r="F85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="H85">
+        <v>28</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
       <c r="F86" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="H86">
+        <v>2</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
       <c r="F87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="H87" t="s">
+        <v>9</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
         <v>7</v>
       </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
       <c r="F88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="H88" t="s">
+        <v>9</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
         <v>3</v>
       </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89">
+        <v>14</v>
+      </c>
+      <c r="E89" t="s">
+        <v>9</v>
+      </c>
       <c r="F89">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="H89">
+        <v>13</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
         <v>5</v>
       </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
       <c r="F90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="H90">
+        <v>60</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
       <c r="F91">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="H91">
+        <v>22</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
         <v>2</v>
       </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92">
+        <v>4</v>
+      </c>
       <c r="F92">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="H92">
+        <v>114</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
       <c r="F93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="H93">
+        <v>112</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
       <c r="F94">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="H94">
+        <v>23</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="s">
+        <v>9</v>
+      </c>
       <c r="F95" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="H95">
+        <v>150</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
       </c>
+      <c r="C96" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96">
+        <v>17</v>
+      </c>
       <c r="F96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="H96">
+        <v>35</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97">
+        <v>12</v>
+      </c>
       <c r="F97">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="H97">
+        <v>34</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" t="s">
+        <v>9</v>
+      </c>
       <c r="F98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="H98" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
         <v>8</v>
       </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
       <c r="F99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="H99">
+        <v>29</v>
+      </c>
+      <c r="I99" t="str">
+        <f>IF(H99&gt;19,"NA",H99+1)</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
       <c r="F100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="H100">
+        <v>70</v>
+      </c>
+      <c r="I100" t="str">
+        <f>IF(H100&gt;19,"NA",H100+1)</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101">
+        <v>12</v>
+      </c>
+      <c r="E101" t="s">
+        <v>9</v>
+      </c>
       <c r="F101" t="s">
         <v>9</v>
+      </c>
+      <c r="H101">
+        <v>11</v>
+      </c>
+      <c r="I101">
+        <f>IF(H101&gt;19,"NA",H101+1)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103">
+        <v>49</v>
+      </c>
+      <c r="C103">
+        <v>84</v>
+      </c>
+      <c r="D103">
+        <v>72</v>
+      </c>
+      <c r="E103">
+        <v>46</v>
+      </c>
+      <c r="F103">
+        <v>42</v>
+      </c>
+      <c r="I103">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>